<commit_message>
reverted changes made back to working v5.5.2 v29 and v4.4.2 v22
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS.xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS.xlsx
@@ -8,29 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9224260-098B-44B8-A32C-D197537BA699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223C9379-AB8B-4E4E-AD33-1E7FA8E60E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13005" yWindow="75" windowWidth="11100" windowHeight="15180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List with Pending or Done" sheetId="1" r:id="rId1"/>
-    <sheet name="Android app version of change" sheetId="2" r:id="rId2"/>
-    <sheet name="Web Server version of change" sheetId="3" r:id="rId3"/>
+    <sheet name="Android app updates Status" sheetId="2" r:id="rId2"/>
+    <sheet name="Web Server updates Status" sheetId="3" r:id="rId3"/>
     <sheet name="Optimized Grouping" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Implemented Changes" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Android app version of change'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Android app updates Status'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'List with Pending or Done'!$A$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Optimized Grouping'!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Web Server version of change'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Web Server updates Status'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="146">
   <si>
     <t>App</t>
   </si>
@@ -366,6 +366,11 @@
   </si>
   <si>
     <t>Admin &amp; Auth</t>
+  </si>
+  <si>
+    <t>• Add server log in admin settings, Tabbed by Server logs, error logs, user logs.  Make downloadable and resettable in gui by starting a new log file.
+• If admin is logged in add "(Admin)" after "Logged In:********" and "User:*****"
+• As admin&gt;Stats: to see who is actively/recently logged in and studying</t>
   </si>
   <si>
     <t>• Add server log in admin settings, Tabbed by Server logs, error logs, user logs.  Make downloadable and resettable in gui by starting a new log file.
@@ -459,13 +464,48 @@
     <t>Bucket for items that don’t match above categories.</t>
   </si>
   <si>
-    <t>• Add server log in admin settings, Tabbed by Server logs, error logs, user logs.  Make downloadable and resettable in gui by starting a new log file.
-• If admin is logged in add "(Admin)" after "Logged In:********" and "User:*****"
-• As admin&gt;Stats: to see who is actively/recently logged in and studying
-• Remove show/hide Custom setting</t>
-  </si>
-  <si>
-    <t>Remember to update readme and changelog, and just update the title of the  Version-****-v*.*.* v**.txt not its content of both projects.  Most recent and complete zip versions are uploaded.  No need to continure providing seperate .md and txt file versions.  Just change in newly updated zip files. Auto choose v1.#.# for Major update, v#.1.# for Medium update, v#.#.1 for minor update.  Remove %20 in zip file names. Update excel with new Fix/Feature Implemented tab when implemented per project.</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Implemented items (Done)</t>
+  </si>
+  <si>
+    <t>2026-01-15</t>
+  </si>
+  <si>
+    <t>Android App</t>
+  </si>
+  <si>
+    <t>Web Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• 
+• 
+• </t>
+  </si>
+  <si>
+    <t>Fixes</t>
+  </si>
+  <si>
+    <t>• In portrait, "Learned" and "All Cards" and "Custom" page Title bar needs to match "Unsure" and "To Study" pages font size and search funtion. In "Learned"&gt;"List" and "Study", remove the redundant status count i.e. "Learned:##" below the other status Counts. On custom page move "Custom:##" in line with the other statuses to the right of "Learned:##"
+•  In landscape, "Learned"&gt;"Study" page needs to match "To Study" and "Unsure" page format design,
+•  In landscape, when search bar opens from spy glass, the text "Search" is cut in half, make text smaller to be seen in box.
+• In landscape, There is unused background space, that can be filled by making cards longer .
+• In both orientations, remove Search bar in all decks; "To Study" (done), "Unsure" (done), "Learned"&gt;"List",  "Learned"&gt;"Study" (Lanscape done, portrait pending), "All" (Lanscape done, portrait pending),  "Custom" (Lanscape done, portrait pending); replace with Spy Glass Icon.  
+• Make "Learned"&gt;"Study" look like other study decks.
+• In search press x to clear search, taping outside of search exits search but keeps results, in settings add random setting for custom study.
+• Saved breakdown text below "Select group..." dropdown does not change on changing cards
+• In "Custom" set status, I dont want the "To Study:###","To Unsure:###","Learned:###" number to reflect the main decks status, but only the custom sets status.  When we select "To Study:###","To Unsure:###","Learned:###" only in custom page it will go to that a custom version of "Unsure" and custom "Learned", custom "Custom:##".  "Custom:##" will show all cards in the Customs set. While in custom page when we tap an action(got it, unsure, learned), cards will only be changed in the custom page not in any main decks or status. Add a Toggle setting Only in Custom page that will push custom Status to main deck if user wants, so when learned in custom deck it will be reflected in main decks.
+• In Custom page, change trash icon function to remove that card only, after confirmation. Change "Remove" button to "Unsure" to move cards to customs Unsure Deck.</t>
   </si>
 </sst>
 </file>
@@ -533,7 +573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -602,11 +642,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -676,8 +727,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -688,6 +745,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1138,16 +1201,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D388"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="90" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" thickBot="1">
@@ -1158,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="38.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:4" ht="57" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1196,7 +1259,7 @@
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="13" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1271,7 @@
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
@@ -1220,7 +1283,7 @@
       <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
@@ -1232,7 +1295,7 @@
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="30"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +1307,7 @@
       <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +1377,7 @@
       <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="12" t="s">
         <v>6</v>
       </c>
@@ -1324,13 +1387,13 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:4" ht="60.75" customHeight="1" thickBot="1">
       <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="15" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1405,7 @@
       <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -1421,7 +1484,7 @@
       <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="28"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="12" t="s">
         <v>6</v>
       </c>
@@ -1433,7 +1496,7 @@
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="30"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="14" t="s">
         <v>8</v>
       </c>
@@ -1445,7 +1508,7 @@
       <c r="A32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="31"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="12" t="s">
         <v>6</v>
       </c>
@@ -2771,7 +2834,7 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -4686,11 +4749,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4717,100 +4780,111 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="150">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:5" ht="409.5">
+      <c r="A2" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="1:5" ht="150">
+      <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="B3" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="C3" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45">
-      <c r="A3" s="26" t="s">
+      <c r="E3" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="26" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="45">
+      <c r="A4" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="B4" s="26" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="375">
-      <c r="A4" s="26" t="s">
+      <c r="C4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="26" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="375">
+      <c r="A5" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="B5" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="C5" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="120">
-      <c r="A5" s="26" t="s">
+      <c r="E5" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="26" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="120">
+      <c r="A6" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26" t="s">
+      <c r="B6" s="26" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>127</v>
-      </c>
       <c r="C6" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="105">
-      <c r="A7" s="26" t="s">
+      <c r="C7" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="26" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="105">
+      <c r="A8" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="B8" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="C8" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="D8" s="26" t="s">
         <v>133</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -4820,21 +4894,63 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534E3D1F-ADED-4C17-A118-30848ED9516B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9000CCF9-7B32-4460-A29C-1EB36984BA73}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="106.5" customHeight="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1" s="19" t="s">
         <v>135</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A2" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A3" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="27" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to new KenpoFlashcardsProject-v4.4.3 v23
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS.xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223C9379-AB8B-4E4E-AD33-1E7FA8E60E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA4CA6C-E270-401A-BD7E-77545566BFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13005" yWindow="75" windowWidth="11100" windowHeight="15180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List with Pending or Done" sheetId="1" r:id="rId1"/>
@@ -496,8 +496,8 @@
     <t>Fixes</t>
   </si>
   <si>
-    <t>• In portrait, "Learned" and "All Cards" and "Custom" page Title bar needs to match "Unsure" and "To Study" pages font size and search funtion. In "Learned"&gt;"List" and "Study", remove the redundant status count i.e. "Learned:##" below the other status Counts. On custom page move "Custom:##" in line with the other statuses to the right of "Learned:##"
-•  In landscape, "Learned"&gt;"Study" page needs to match "To Study" and "Unsure" page format design,
+    <t xml:space="preserve">• In portrait, "Learned" and "All Cards" and "Custom" page Title bar needs to match "Unsure" and "To Study" pages smaller font size and search funtion with Magnifying Glass. In "Learned"&gt;"List" and "Study", remove the redundant status count i.e. "Learned:##" below the other status Counts. On custom page move "Custom:##" in line with the "Card#/#" to the left.
+•  In landscape, "Learned"&gt;"Study" and "Custom" page needs to match "To Study" and "Unsure" page format design, change trash icon function to remove that card only, after confirmation. Change "Remove" button to "Unsure" to move cards to customs Unsure Deck.
 •  In landscape, when search bar opens from spy glass, the text "Search" is cut in half, make text smaller to be seen in box.
 • In landscape, There is unused background space, that can be filled by making cards longer .
 • In both orientations, remove Search bar in all decks; "To Study" (done), "Unsure" (done), "Learned"&gt;"List",  "Learned"&gt;"Study" (Lanscape done, portrait pending), "All" (Lanscape done, portrait pending),  "Custom" (Lanscape done, portrait pending); replace with Spy Glass Icon.  
@@ -505,7 +505,7 @@
 • In search press x to clear search, taping outside of search exits search but keeps results, in settings add random setting for custom study.
 • Saved breakdown text below "Select group..." dropdown does not change on changing cards
 • In "Custom" set status, I dont want the "To Study:###","To Unsure:###","Learned:###" number to reflect the main decks status, but only the custom sets status.  When we select "To Study:###","To Unsure:###","Learned:###" only in custom page it will go to that a custom version of "Unsure" and custom "Learned", custom "Custom:##".  "Custom:##" will show all cards in the Customs set. While in custom page when we tap an action(got it, unsure, learned), cards will only be changed in the custom page not in any main decks or status. Add a Toggle setting Only in Custom page that will push custom Status to main deck if user wants, so when learned in custom deck it will be reflected in main decks.
-• In Custom page, change trash icon function to remove that card only, after confirmation. Change "Remove" button to "Unsure" to move cards to customs Unsure Deck.</t>
+</t>
   </si>
 </sst>
 </file>
@@ -657,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -736,6 +736,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -746,11 +752,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1201,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D388"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1259,7 +1268,7 @@
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="13" t="s">
         <v>8</v>
       </c>
@@ -1271,7 +1280,7 @@
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
@@ -1283,7 +1292,7 @@
       <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
@@ -1295,7 +1304,7 @@
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
@@ -1307,7 +1316,7 @@
       <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
@@ -1377,7 +1386,7 @@
       <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="30"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="12" t="s">
         <v>6</v>
       </c>
@@ -1387,13 +1396,13 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="31"/>
+      <c r="B18" s="33"/>
     </row>
     <row r="19" spans="1:4" ht="60.75" customHeight="1" thickBot="1">
       <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="15" t="s">
         <v>8</v>
       </c>
@@ -1405,7 +1414,7 @@
       <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -1484,7 +1493,7 @@
       <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="12" t="s">
         <v>6</v>
       </c>
@@ -1496,7 +1505,7 @@
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="14" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1517,7 @@
       <c r="A32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="12" t="s">
         <v>6</v>
       </c>
@@ -4751,20 +4760,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="4" width="55" customWidth="1"/>
+    <col min="1" max="1" width="22" style="38" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" customWidth="1"/>
+    <col min="3" max="4" width="55" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="36" t="s">
         <v>106</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -4780,11 +4790,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:5" ht="375">
+      <c r="A2" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="31" t="s">
         <v>145</v>
       </c>
       <c r="C2" s="26"/>
@@ -4792,7 +4802,7 @@
       <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="150">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="37" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -4809,7 +4819,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="37" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -4823,8 +4833,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="375">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:5" ht="285">
+      <c r="A5" s="37" t="s">
         <v>119</v>
       </c>
       <c r="B5" s="26" t="s">
@@ -4841,7 +4851,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="120">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="37" t="s">
         <v>124</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -4856,7 +4866,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="37" t="s">
         <v>127</v>
       </c>
       <c r="B7" s="26" t="s">
@@ -4871,7 +4881,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="105">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="37" t="s">
         <v>130</v>
       </c>
       <c r="B8" s="26" t="s">

</xml_diff>